<commit_message>
Atualizaçao do ficheiro de tarefas.xls
</commit_message>
<xml_diff>
--- a/Documentação/tarefas.xlsx
+++ b/Documentação/tarefas.xlsx
@@ -183,7 +183,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -202,6 +202,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="7">
     <border>
@@ -291,7 +303,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -312,78 +324,108 @@
       <alignment vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -668,14 +710,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="62" style="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62" style="15" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
@@ -687,21 +729,21 @@
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="8" t="s">
+      <c r="B2" s="10"/>
+      <c r="C2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="11" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -724,330 +766,330 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="7" t="s">
         <v>21</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D4" s="2"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-    </row>
-    <row r="5" spans="1:8" s="28" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="27" t="s">
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+    </row>
+    <row r="5" spans="1:8" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="23"/>
+      <c r="B5" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-    </row>
-    <row r="6" spans="1:8" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="27" t="s">
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+    </row>
+    <row r="6" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="23"/>
+      <c r="B6" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-    </row>
-    <row r="7" spans="1:8" s="28" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="27" t="s">
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+    </row>
+    <row r="7" spans="1:8" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="23"/>
+      <c r="B7" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
-    </row>
-    <row r="8" spans="1:8" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
-      <c r="B8" s="27" t="s">
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+    </row>
+    <row r="8" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="23"/>
+      <c r="B8" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
     </row>
     <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="10" t="s">
+      <c r="A9" s="23"/>
+      <c r="B9" s="7" t="s">
         <v>26</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" s="24"/>
-      <c r="H9" s="24"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-      <c r="B10" s="10" t="s">
+      <c r="A10" s="23"/>
+      <c r="B10" s="7" t="s">
         <v>27</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" s="24"/>
-      <c r="H10" s="24"/>
-    </row>
-    <row r="11" spans="1:8" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="27" t="s">
+      <c r="E10" s="17"/>
+      <c r="F10" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+    </row>
+    <row r="11" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="23"/>
+      <c r="B11" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
-    </row>
-    <row r="12" spans="1:8" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="27" t="s">
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+    </row>
+    <row r="12" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="23"/>
+      <c r="B12" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
-    </row>
-    <row r="13" spans="1:8" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="27" t="s">
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+    </row>
+    <row r="13" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="23"/>
+      <c r="B13" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="B14" s="10" t="s">
+      <c r="A14" s="23"/>
+      <c r="B14" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
     </row>
     <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="16"/>
-      <c r="B15" s="19"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
+      <c r="A15" s="24"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
     </row>
     <row r="16" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
-      <c r="B17" s="10" t="s">
+      <c r="C16" s="8"/>
+      <c r="D16" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+    </row>
+    <row r="17" spans="1:8" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="27"/>
+      <c r="B17" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17" s="2"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="24"/>
-    </row>
-    <row r="18" spans="1:8" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
-      <c r="B18" s="27" t="s">
+      <c r="C17" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+    </row>
+    <row r="18" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="27"/>
+      <c r="B18" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="23"/>
-      <c r="H18" s="23"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="9"/>
-      <c r="B19" s="10" t="s">
+      <c r="A19" s="27"/>
+      <c r="B19" s="7" t="s">
         <v>20</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="24"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
     </row>
     <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="12"/>
-      <c r="B20" s="19" t="s">
+      <c r="A20" s="28"/>
+      <c r="B20" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="F20" s="25"/>
-      <c r="G20" s="25"/>
-      <c r="H20" s="25"/>
-    </row>
-    <row r="21" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+    </row>
+    <row r="21" spans="1:8" s="32" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="H21" s="26"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
-      <c r="B22" s="10" t="s">
+      <c r="C21" s="31"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="H21" s="31"/>
+    </row>
+    <row r="22" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="23"/>
+      <c r="B22" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="H22" s="24"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="H22" s="34"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
-      <c r="B23" s="10" t="s">
+      <c r="A23" s="23"/>
+      <c r="B23" s="7" t="s">
         <v>34</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
-      <c r="E23" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="F23" s="24"/>
-      <c r="G23" s="24"/>
-      <c r="H23" s="24"/>
+      <c r="E23" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
-      <c r="B24" s="10" t="s">
+      <c r="A24" s="23"/>
+      <c r="B24" s="7" t="s">
         <v>35</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E24" s="24"/>
-      <c r="F24" s="24"/>
-      <c r="G24" s="24"/>
-      <c r="H24" s="24"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
-      <c r="B25" s="10" t="s">
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
+    </row>
+    <row r="25" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="23"/>
+      <c r="B25" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="24"/>
-      <c r="G25" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="H25" s="24"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
-      <c r="B26" s="10" t="s">
+      <c r="C25" s="34"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="34"/>
+      <c r="G25" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="H25" s="34"/>
+    </row>
+    <row r="26" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="23"/>
+      <c r="B26" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="24"/>
-      <c r="G26" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="H26" s="24"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
-      <c r="B27" s="10" t="s">
+      <c r="C26" s="34"/>
+      <c r="D26" s="34"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="34"/>
+      <c r="G26" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="H26" s="34"/>
+    </row>
+    <row r="27" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="23"/>
+      <c r="B27" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D27" s="2"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
+      <c r="C27" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" s="34"/>
+      <c r="E27" s="34"/>
+      <c r="F27" s="34"/>
+      <c r="G27" s="34"/>
+      <c r="H27" s="34"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
-      <c r="B28" s="10" t="s">
+      <c r="A28" s="23"/>
+      <c r="B28" s="7" t="s">
         <v>40</v>
       </c>
       <c r="C28" s="2" t="s">
@@ -1059,129 +1101,129 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="7"/>
-      <c r="B29" s="10" t="s">
+    <row r="29" spans="1:8" s="32" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="23"/>
+      <c r="B29" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="7"/>
-      <c r="B30" s="10" t="s">
+      <c r="C29" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29" s="34"/>
+      <c r="E29" s="34"/>
+      <c r="F29" s="34"/>
+      <c r="G29" s="34"/>
+      <c r="H29" s="34"/>
+    </row>
+    <row r="30" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="23"/>
+      <c r="B30" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
-      <c r="B31" s="10" t="s">
+      <c r="C30" s="34"/>
+      <c r="D30" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" s="34"/>
+      <c r="F30" s="34"/>
+      <c r="G30" s="34"/>
+      <c r="H30" s="34"/>
+    </row>
+    <row r="31" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="23"/>
+      <c r="B31" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="7"/>
-      <c r="B32" s="10" t="s">
+      <c r="C31" s="34"/>
+      <c r="D31" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="E31" s="34"/>
+      <c r="F31" s="34"/>
+      <c r="G31" s="34"/>
+      <c r="H31" s="34"/>
+    </row>
+    <row r="32" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="23"/>
+      <c r="B32" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C32" s="34"/>
+      <c r="D32" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" s="34"/>
+      <c r="F32" s="34"/>
+      <c r="G32" s="34"/>
+      <c r="H32" s="34"/>
+    </row>
+    <row r="33" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="29"/>
-      <c r="B33" s="30" t="s">
+      <c r="B33" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="C33" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="D33" s="31"/>
-      <c r="E33" s="31"/>
-      <c r="F33" s="31"/>
-      <c r="G33" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="H33" s="31"/>
-    </row>
-    <row r="34" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="16"/>
-      <c r="B34" s="19" t="s">
+      <c r="C33" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="D33" s="36"/>
+      <c r="E33" s="36"/>
+      <c r="F33" s="36"/>
+      <c r="G33" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="H33" s="36"/>
+    </row>
+    <row r="34" spans="1:10" s="32" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="24"/>
+      <c r="B34" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C34" s="14"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="14"/>
-      <c r="G34" s="14"/>
-      <c r="H34" s="14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="25.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="11" t="s">
+      <c r="C34" s="38"/>
+      <c r="D34" s="38"/>
+      <c r="E34" s="38"/>
+      <c r="F34" s="38"/>
+      <c r="G34" s="38"/>
+      <c r="H34" s="38" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" s="32" customFormat="1" ht="25.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="B35" s="20" t="s">
+      <c r="B35" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H35" s="13"/>
-    </row>
-    <row r="36" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="7"/>
-      <c r="B36" s="10" t="s">
+      <c r="C35" s="31"/>
+      <c r="D35" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35" s="31"/>
+      <c r="F35" s="31"/>
+      <c r="G35" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="H35" s="31"/>
+    </row>
+    <row r="36" spans="1:10" s="32" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="23"/>
+      <c r="B36" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H36" s="2"/>
+      <c r="C36" s="34"/>
+      <c r="D36" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
+      <c r="G36" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="H36" s="34"/>
     </row>
     <row r="37" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="7"/>
-      <c r="B37" s="10" t="s">
+      <c r="A37" s="23"/>
+      <c r="B37" s="7" t="s">
         <v>16</v>
       </c>
       <c r="C37" s="2"/>
@@ -1194,8 +1236,8 @@
       <c r="H37" s="2"/>
     </row>
     <row r="38" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="7"/>
-      <c r="B38" s="10" t="s">
+      <c r="A38" s="23"/>
+      <c r="B38" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C38" s="2"/>
@@ -1208,18 +1250,18 @@
       <c r="H38" s="2"/>
     </row>
     <row r="39" spans="1:10" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="16"/>
-      <c r="B39" s="19"/>
-      <c r="C39" s="14"/>
-      <c r="D39" s="14"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="14"/>
-      <c r="G39" s="14"/>
-      <c r="H39" s="14"/>
+      <c r="A39" s="24"/>
+      <c r="B39" s="12"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="9"/>
+      <c r="H39" s="9"/>
     </row>
     <row r="40" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A40" s="6"/>
-      <c r="B40" s="21"/>
+      <c r="B40" s="14"/>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
@@ -1231,7 +1273,7 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="6"/>
-      <c r="B41" s="21"/>
+      <c r="B41" s="14"/>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
@@ -1243,7 +1285,7 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="6"/>
-      <c r="B42" s="21"/>
+      <c r="B42" s="14"/>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
@@ -1255,7 +1297,7 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="6"/>
-      <c r="B43" s="21"/>
+      <c r="B43" s="14"/>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
@@ -1267,7 +1309,7 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="5"/>
-      <c r="B44" s="21"/>
+      <c r="B44" s="14"/>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>

</xml_diff>

<commit_message>
Conversao da distribuiçao de tarefas para jpeg
</commit_message>
<xml_diff>
--- a/Documentação/tarefas.xlsx
+++ b/Documentação/tarefas.xlsx
@@ -210,7 +210,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -368,6 +368,33 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -391,33 +418,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -710,8 +710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -730,14 +730,14 @@
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="10"/>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -766,7 +766,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="32" t="s">
         <v>44</v>
       </c>
       <c r="B4" s="7" t="s">
@@ -782,7 +782,7 @@
       <c r="H4" s="17"/>
     </row>
     <row r="5" spans="1:8" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="23"/>
+      <c r="A5" s="32"/>
       <c r="B5" s="20" t="s">
         <v>22</v>
       </c>
@@ -794,7 +794,7 @@
       <c r="H5" s="16"/>
     </row>
     <row r="6" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="23"/>
+      <c r="A6" s="32"/>
       <c r="B6" s="20" t="s">
         <v>23</v>
       </c>
@@ -806,7 +806,7 @@
       <c r="H6" s="16"/>
     </row>
     <row r="7" spans="1:8" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="23"/>
+      <c r="A7" s="32"/>
       <c r="B7" s="20" t="s">
         <v>24</v>
       </c>
@@ -818,7 +818,7 @@
       <c r="H7" s="16"/>
     </row>
     <row r="8" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="23"/>
+      <c r="A8" s="32"/>
       <c r="B8" s="20" t="s">
         <v>25</v>
       </c>
@@ -830,7 +830,7 @@
       <c r="H8" s="16"/>
     </row>
     <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="23"/>
+      <c r="A9" s="32"/>
       <c r="B9" s="7" t="s">
         <v>26</v>
       </c>
@@ -844,7 +844,7 @@
       <c r="H9" s="17"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="23"/>
+      <c r="A10" s="32"/>
       <c r="B10" s="7" t="s">
         <v>27</v>
       </c>
@@ -858,7 +858,7 @@
       <c r="H10" s="17"/>
     </row>
     <row r="11" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="23"/>
+      <c r="A11" s="32"/>
       <c r="B11" s="20" t="s">
         <v>28</v>
       </c>
@@ -869,20 +869,20 @@
       <c r="G11" s="16"/>
       <c r="H11" s="16"/>
     </row>
-    <row r="12" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="23"/>
-      <c r="B12" s="20" t="s">
+    <row r="12" spans="1:8" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="32"/>
+      <c r="B12" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="40"/>
     </row>
     <row r="13" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="23"/>
+      <c r="A13" s="32"/>
       <c r="B13" s="20" t="s">
         <v>30</v>
       </c>
@@ -894,7 +894,7 @@
       <c r="H13" s="16"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="23"/>
+      <c r="A14" s="32"/>
       <c r="B14" s="7" t="s">
         <v>31</v>
       </c>
@@ -908,7 +908,7 @@
       <c r="H14" s="17"/>
     </row>
     <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="24"/>
+      <c r="A15" s="33"/>
       <c r="B15" s="12"/>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
@@ -918,7 +918,7 @@
       <c r="H15" s="18"/>
     </row>
     <row r="16" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="35" t="s">
         <v>9</v>
       </c>
       <c r="B16" s="13" t="s">
@@ -934,7 +934,7 @@
       <c r="H16" s="19"/>
     </row>
     <row r="17" spans="1:8" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="27"/>
+      <c r="A17" s="36"/>
       <c r="B17" s="39" t="s">
         <v>18</v>
       </c>
@@ -948,7 +948,7 @@
       <c r="H17" s="40"/>
     </row>
     <row r="18" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="27"/>
+      <c r="A18" s="36"/>
       <c r="B18" s="20" t="s">
         <v>19</v>
       </c>
@@ -960,7 +960,7 @@
       <c r="H18" s="16"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="27"/>
+      <c r="A19" s="36"/>
       <c r="B19" s="7" t="s">
         <v>20</v>
       </c>
@@ -974,7 +974,7 @@
       <c r="H19" s="17"/>
     </row>
     <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="28"/>
+      <c r="A20" s="37"/>
       <c r="B20" s="12" t="s">
         <v>45</v>
       </c>
@@ -987,38 +987,38 @@
       <c r="G20" s="18"/>
       <c r="H20" s="18"/>
     </row>
-    <row r="21" spans="1:8" s="32" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="22" t="s">
+    <row r="21" spans="1:8" s="24" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="30" t="s">
+      <c r="B21" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="31"/>
-      <c r="G21" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="H21" s="31"/>
-    </row>
-    <row r="22" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="23"/>
-      <c r="B22" s="33" t="s">
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="H21" s="23"/>
+    </row>
+    <row r="22" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="32"/>
+      <c r="B22" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="C22" s="34"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="34"/>
-      <c r="G22" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="H22" s="34"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="H22" s="26"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="23"/>
+      <c r="A23" s="32"/>
       <c r="B23" s="7" t="s">
         <v>34</v>
       </c>
@@ -1032,7 +1032,7 @@
       <c r="H23" s="17"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="23"/>
+      <c r="A24" s="32"/>
       <c r="B24" s="7" t="s">
         <v>35</v>
       </c>
@@ -1045,50 +1045,50 @@
       <c r="G24" s="17"/>
       <c r="H24" s="17"/>
     </row>
-    <row r="25" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="23"/>
-      <c r="B25" s="33" t="s">
+    <row r="25" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="32"/>
+      <c r="B25" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="34"/>
-      <c r="D25" s="34"/>
-      <c r="E25" s="34"/>
-      <c r="F25" s="34"/>
-      <c r="G25" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="H25" s="34"/>
-    </row>
-    <row r="26" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="23"/>
-      <c r="B26" s="33" t="s">
+      <c r="C25" s="26"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="H25" s="26"/>
+    </row>
+    <row r="26" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="32"/>
+      <c r="B26" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="C26" s="34"/>
-      <c r="D26" s="34"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34"/>
-      <c r="G26" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="H26" s="34"/>
-    </row>
-    <row r="27" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="23"/>
-      <c r="B27" s="33" t="s">
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="H26" s="26"/>
+    </row>
+    <row r="27" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="32"/>
+      <c r="B27" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="C27" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="D27" s="34"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="34"/>
-      <c r="H27" s="34"/>
+      <c r="C27" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="26"/>
+      <c r="G27" s="26"/>
+      <c r="H27" s="26"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="23"/>
+      <c r="A28" s="32"/>
       <c r="B28" s="7" t="s">
         <v>40</v>
       </c>
@@ -1101,142 +1101,142 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" s="32" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="23"/>
-      <c r="B29" s="33" t="s">
+    <row r="29" spans="1:8" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="32"/>
+      <c r="B29" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="C29" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="D29" s="34"/>
-      <c r="E29" s="34"/>
-      <c r="F29" s="34"/>
-      <c r="G29" s="34"/>
-      <c r="H29" s="34"/>
-    </row>
-    <row r="30" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="23"/>
-      <c r="B30" s="33" t="s">
+      <c r="C29" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+    </row>
+    <row r="30" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="32"/>
+      <c r="B30" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="C30" s="34"/>
-      <c r="D30" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="E30" s="34"/>
-      <c r="F30" s="34"/>
-      <c r="G30" s="34"/>
-      <c r="H30" s="34"/>
-    </row>
-    <row r="31" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="23"/>
-      <c r="B31" s="33" t="s">
+      <c r="C30" s="26"/>
+      <c r="D30" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="26"/>
+    </row>
+    <row r="31" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="32"/>
+      <c r="B31" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="C31" s="34"/>
-      <c r="D31" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="E31" s="34"/>
-      <c r="F31" s="34"/>
-      <c r="G31" s="34"/>
-      <c r="H31" s="34"/>
-    </row>
-    <row r="32" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="23"/>
-      <c r="B32" s="33" t="s">
+      <c r="C31" s="26"/>
+      <c r="D31" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="E31" s="26"/>
+      <c r="F31" s="26"/>
+      <c r="G31" s="26"/>
+      <c r="H31" s="26"/>
+    </row>
+    <row r="32" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="32"/>
+      <c r="B32" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="C32" s="34"/>
-      <c r="D32" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="E32" s="34"/>
-      <c r="F32" s="34"/>
-      <c r="G32" s="34"/>
-      <c r="H32" s="34"/>
-    </row>
-    <row r="33" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="29"/>
-      <c r="B33" s="35" t="s">
+      <c r="C32" s="26"/>
+      <c r="D32" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" s="26"/>
+      <c r="F32" s="26"/>
+      <c r="G32" s="26"/>
+      <c r="H32" s="26"/>
+    </row>
+    <row r="33" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="38"/>
+      <c r="B33" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="C33" s="36" t="s">
-        <v>12</v>
-      </c>
-      <c r="D33" s="36"/>
-      <c r="E33" s="36"/>
-      <c r="F33" s="36"/>
-      <c r="G33" s="36" t="s">
-        <v>12</v>
-      </c>
-      <c r="H33" s="36"/>
-    </row>
-    <row r="34" spans="1:10" s="32" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="24"/>
-      <c r="B34" s="37" t="s">
+      <c r="C33" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="D33" s="28"/>
+      <c r="E33" s="28"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="H33" s="28"/>
+    </row>
+    <row r="34" spans="1:10" s="24" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="33"/>
+      <c r="B34" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="C34" s="38"/>
-      <c r="D34" s="38"/>
-      <c r="E34" s="38"/>
-      <c r="F34" s="38"/>
-      <c r="G34" s="38"/>
-      <c r="H34" s="38" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" s="32" customFormat="1" ht="25.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="22" t="s">
+      <c r="C34" s="30"/>
+      <c r="D34" s="30"/>
+      <c r="E34" s="30"/>
+      <c r="F34" s="30"/>
+      <c r="G34" s="30"/>
+      <c r="H34" s="30" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" s="24" customFormat="1" ht="25.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="B35" s="30" t="s">
+      <c r="B35" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="C35" s="31"/>
-      <c r="D35" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="E35" s="31"/>
-      <c r="F35" s="31"/>
-      <c r="G35" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="H35" s="31"/>
-    </row>
-    <row r="36" spans="1:10" s="32" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="23"/>
-      <c r="B36" s="33" t="s">
+      <c r="C35" s="23"/>
+      <c r="D35" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35" s="23"/>
+      <c r="F35" s="23"/>
+      <c r="G35" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="H35" s="23"/>
+    </row>
+    <row r="36" spans="1:10" s="24" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="32"/>
+      <c r="B36" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="C36" s="34"/>
-      <c r="D36" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
-      <c r="G36" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="H36" s="34"/>
-    </row>
-    <row r="37" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="23"/>
-      <c r="B37" s="7" t="s">
+      <c r="C36" s="26"/>
+      <c r="D36" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="E36" s="26"/>
+      <c r="F36" s="26"/>
+      <c r="G36" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="H36" s="26"/>
+    </row>
+    <row r="37" spans="1:10" s="41" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="32"/>
+      <c r="B37" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H37" s="2"/>
+      <c r="C37" s="40"/>
+      <c r="D37" s="40"/>
+      <c r="E37" s="40"/>
+      <c r="F37" s="40"/>
+      <c r="G37" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="H37" s="40"/>
     </row>
     <row r="38" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="23"/>
+      <c r="A38" s="32"/>
       <c r="B38" s="7" t="s">
         <v>17</v>
       </c>
@@ -1250,7 +1250,7 @@
       <c r="H38" s="2"/>
     </row>
     <row r="39" spans="1:10" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="24"/>
+      <c r="A39" s="33"/>
       <c r="B39" s="12"/>
       <c r="C39" s="9"/>
       <c r="D39" s="9"/>

</xml_diff>

<commit_message>
alterado ficheiro de planeamento de tarefas para as tarefas finais
</commit_message>
<xml_diff>
--- a/Documentação/tarefas.xlsx
+++ b/Documentação/tarefas.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LAPR\Documentação\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DEV\Projects\easySoft\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="51">
   <si>
     <t>Módulo</t>
   </si>
@@ -168,14 +168,31 @@
   </si>
   <si>
     <t>webservice forca</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>webservice distribuicao de dados</t>
+  </si>
+  <si>
+    <t>cliente de login e launcher</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -303,7 +320,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -395,6 +412,15 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -419,13 +445,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -708,10 +728,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J44"/>
+  <dimension ref="A2:J45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B12" sqref="A12:XFD12"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -730,14 +750,14 @@
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="10"/>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -766,7 +786,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="35" t="s">
         <v>44</v>
       </c>
       <c r="B4" s="7" t="s">
@@ -782,7 +802,7 @@
       <c r="H4" s="17"/>
     </row>
     <row r="5" spans="1:8" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="32"/>
+      <c r="A5" s="35"/>
       <c r="B5" s="20" t="s">
         <v>22</v>
       </c>
@@ -794,7 +814,7 @@
       <c r="H5" s="16"/>
     </row>
     <row r="6" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="32"/>
+      <c r="A6" s="35"/>
       <c r="B6" s="20" t="s">
         <v>23</v>
       </c>
@@ -806,7 +826,7 @@
       <c r="H6" s="16"/>
     </row>
     <row r="7" spans="1:8" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="32"/>
+      <c r="A7" s="35"/>
       <c r="B7" s="20" t="s">
         <v>24</v>
       </c>
@@ -818,7 +838,7 @@
       <c r="H7" s="16"/>
     </row>
     <row r="8" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="32"/>
+      <c r="A8" s="35"/>
       <c r="B8" s="20" t="s">
         <v>25</v>
       </c>
@@ -830,7 +850,7 @@
       <c r="H8" s="16"/>
     </row>
     <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="32"/>
+      <c r="A9" s="35"/>
       <c r="B9" s="7" t="s">
         <v>26</v>
       </c>
@@ -844,7 +864,7 @@
       <c r="H9" s="17"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="32"/>
+      <c r="A10" s="35"/>
       <c r="B10" s="7" t="s">
         <v>27</v>
       </c>
@@ -858,7 +878,7 @@
       <c r="H10" s="17"/>
     </row>
     <row r="11" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="32"/>
+      <c r="A11" s="35"/>
       <c r="B11" s="20" t="s">
         <v>28</v>
       </c>
@@ -869,20 +889,24 @@
       <c r="G11" s="16"/>
       <c r="H11" s="16"/>
     </row>
-    <row r="12" spans="1:8" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="32"/>
-      <c r="B12" s="39" t="s">
+    <row r="12" spans="1:8" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="35"/>
+      <c r="B12" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="40"/>
-      <c r="D12" s="40"/>
-      <c r="E12" s="40"/>
-      <c r="F12" s="40"/>
-      <c r="G12" s="40"/>
-      <c r="H12" s="40"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="13" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="32"/>
+      <c r="A13" s="35"/>
       <c r="B13" s="20" t="s">
         <v>30</v>
       </c>
@@ -894,31 +918,35 @@
       <c r="H13" s="16"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="32"/>
+      <c r="A14" s="35"/>
       <c r="B14" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="17"/>
-      <c r="F14" s="17" t="s">
-        <v>12</v>
-      </c>
+      <c r="F14" s="17"/>
       <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
+      <c r="H14" s="17" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="33"/>
-      <c r="B15" s="12"/>
+      <c r="A15" s="36"/>
+      <c r="B15" s="12" t="s">
+        <v>50</v>
+      </c>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
       <c r="E15" s="18"/>
       <c r="F15" s="18"/>
       <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
+      <c r="H15" s="18" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="16" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="38" t="s">
         <v>9</v>
       </c>
       <c r="B16" s="13" t="s">
@@ -933,22 +961,22 @@
       <c r="G16" s="19"/>
       <c r="H16" s="19"/>
     </row>
-    <row r="17" spans="1:8" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="36"/>
-      <c r="B17" s="39" t="s">
+    <row r="17" spans="1:8" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="39"/>
+      <c r="B17" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="40" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17" s="40"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="40"/>
+      <c r="C17" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
     </row>
     <row r="18" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="36"/>
+      <c r="A18" s="39"/>
       <c r="B18" s="20" t="s">
         <v>19</v>
       </c>
@@ -960,7 +988,7 @@
       <c r="H18" s="16"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="36"/>
+      <c r="A19" s="39"/>
       <c r="B19" s="7" t="s">
         <v>20</v>
       </c>
@@ -974,7 +1002,7 @@
       <c r="H19" s="17"/>
     </row>
     <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="37"/>
+      <c r="A20" s="40"/>
       <c r="B20" s="12" t="s">
         <v>45</v>
       </c>
@@ -988,7 +1016,7 @@
       <c r="H20" s="18"/>
     </row>
     <row r="21" spans="1:8" s="24" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="31" t="s">
+      <c r="A21" s="34" t="s">
         <v>10</v>
       </c>
       <c r="B21" s="22" t="s">
@@ -1004,7 +1032,7 @@
       <c r="H21" s="23"/>
     </row>
     <row r="22" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="32"/>
+      <c r="A22" s="35"/>
       <c r="B22" s="25" t="s">
         <v>33</v>
       </c>
@@ -1018,7 +1046,7 @@
       <c r="H22" s="26"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="32"/>
+      <c r="A23" s="35"/>
       <c r="B23" s="7" t="s">
         <v>34</v>
       </c>
@@ -1032,7 +1060,7 @@
       <c r="H23" s="17"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="32"/>
+      <c r="A24" s="35"/>
       <c r="B24" s="7" t="s">
         <v>35</v>
       </c>
@@ -1046,7 +1074,7 @@
       <c r="H24" s="17"/>
     </row>
     <row r="25" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="32"/>
+      <c r="A25" s="35"/>
       <c r="B25" s="25" t="s">
         <v>36</v>
       </c>
@@ -1060,7 +1088,7 @@
       <c r="H25" s="26"/>
     </row>
     <row r="26" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="32"/>
+      <c r="A26" s="35"/>
       <c r="B26" s="25" t="s">
         <v>37</v>
       </c>
@@ -1074,7 +1102,7 @@
       <c r="H26" s="26"/>
     </row>
     <row r="27" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="32"/>
+      <c r="A27" s="35"/>
       <c r="B27" s="25" t="s">
         <v>38</v>
       </c>
@@ -1088,7 +1116,7 @@
       <c r="H27" s="26"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="32"/>
+      <c r="A28" s="35"/>
       <c r="B28" s="7" t="s">
         <v>40</v>
       </c>
@@ -1102,7 +1130,7 @@
       <c r="H28" s="2"/>
     </row>
     <row r="29" spans="1:8" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="32"/>
+      <c r="A29" s="35"/>
       <c r="B29" s="25" t="s">
         <v>39</v>
       </c>
@@ -1116,7 +1144,7 @@
       <c r="H29" s="26"/>
     </row>
     <row r="30" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="32"/>
+      <c r="A30" s="35"/>
       <c r="B30" s="25" t="s">
         <v>41</v>
       </c>
@@ -1130,7 +1158,7 @@
       <c r="H30" s="26"/>
     </row>
     <row r="31" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="32"/>
+      <c r="A31" s="35"/>
       <c r="B31" s="25" t="s">
         <v>42</v>
       </c>
@@ -1138,13 +1166,13 @@
       <c r="D31" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="E31" s="26"/>
+      <c r="E31" s="42"/>
       <c r="F31" s="26"/>
       <c r="G31" s="26"/>
       <c r="H31" s="26"/>
     </row>
     <row r="32" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="32"/>
+      <c r="A32" s="35"/>
       <c r="B32" s="25" t="s">
         <v>43</v>
       </c>
@@ -1158,120 +1186,124 @@
       <c r="H32" s="26"/>
     </row>
     <row r="33" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="38"/>
+      <c r="A33" s="41"/>
       <c r="B33" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="C33" s="28" t="s">
-        <v>12</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="C33" s="28"/>
       <c r="D33" s="28"/>
       <c r="E33" s="28"/>
       <c r="F33" s="28"/>
-      <c r="G33" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="H33" s="28"/>
-    </row>
-    <row r="34" spans="1:10" s="24" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="33"/>
-      <c r="B34" s="29" t="s">
+      <c r="G33" s="28"/>
+      <c r="H33" s="28" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="41"/>
+      <c r="B34" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="C34" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="D34" s="28"/>
+      <c r="E34" s="28"/>
+      <c r="F34" s="28"/>
+      <c r="G34" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="H34" s="28" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" s="24" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="36"/>
+      <c r="B35" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="C34" s="30"/>
-      <c r="D34" s="30"/>
-      <c r="E34" s="30"/>
-      <c r="F34" s="30"/>
-      <c r="G34" s="30"/>
-      <c r="H34" s="30" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" s="24" customFormat="1" ht="25.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="31" t="s">
+      <c r="C35" s="30"/>
+      <c r="D35" s="30"/>
+      <c r="E35" s="30"/>
+      <c r="F35" s="30"/>
+      <c r="G35" s="30"/>
+      <c r="H35" s="30" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" s="24" customFormat="1" ht="25.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="B35" s="22" t="s">
+      <c r="B36" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="C35" s="23"/>
-      <c r="D35" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23"/>
-      <c r="G35" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="H35" s="23"/>
-    </row>
-    <row r="36" spans="1:10" s="24" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="32"/>
-      <c r="B36" s="25" t="s">
+      <c r="C36" s="23"/>
+      <c r="D36" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="E36" s="23"/>
+      <c r="F36" s="23"/>
+      <c r="G36" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="H36" s="23"/>
+    </row>
+    <row r="37" spans="1:10" s="24" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="35"/>
+      <c r="B37" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="C36" s="26"/>
-      <c r="D36" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="E36" s="26"/>
-      <c r="F36" s="26"/>
-      <c r="G36" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="H36" s="26"/>
-    </row>
-    <row r="37" spans="1:10" s="41" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="32"/>
-      <c r="B37" s="39" t="s">
+      <c r="C37" s="26"/>
+      <c r="D37" s="26"/>
+      <c r="E37" s="26"/>
+      <c r="F37" s="26"/>
+      <c r="G37" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="H37" s="26" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" s="33" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="35"/>
+      <c r="B38" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="C37" s="40"/>
-      <c r="D37" s="40"/>
-      <c r="E37" s="40"/>
-      <c r="F37" s="40"/>
-      <c r="G37" s="40" t="s">
-        <v>12</v>
-      </c>
-      <c r="H37" s="40"/>
-    </row>
-    <row r="38" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="32"/>
-      <c r="B38" s="7" t="s">
+      <c r="C38" s="32"/>
+      <c r="D38" s="32"/>
+      <c r="E38" s="32"/>
+      <c r="F38" s="32"/>
+      <c r="G38" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="H38" s="32"/>
+    </row>
+    <row r="39" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="35"/>
+      <c r="B39" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
-    </row>
-    <row r="39" spans="1:10" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="33"/>
-      <c r="B39" s="12"/>
-      <c r="C39" s="9"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="9"/>
-      <c r="G39" s="9"/>
-      <c r="H39" s="9"/>
-    </row>
-    <row r="40" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="6"/>
-      <c r="B40" s="14"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="5"/>
-      <c r="F40" s="5"/>
-      <c r="G40" s="5"/>
-      <c r="H40" s="5"/>
-      <c r="I40" s="5"/>
-      <c r="J40" s="5"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+    </row>
+    <row r="40" spans="1:10" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="36"/>
+      <c r="B40" s="12"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
+    </row>
+    <row r="41" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A41" s="6"/>
       <c r="B41" s="14"/>
       <c r="C41" s="5"/>
@@ -1308,7 +1340,7 @@
       <c r="J43" s="5"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="5"/>
+      <c r="A44" s="6"/>
       <c r="B44" s="14"/>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
@@ -1319,13 +1351,25 @@
       <c r="I44" s="5"/>
       <c r="J44" s="5"/>
     </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="5"/>
+      <c r="B45" s="14"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="5"/>
+      <c r="I45" s="5"/>
+      <c r="J45" s="5"/>
+    </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="A35:A39"/>
+    <mergeCell ref="A36:A40"/>
     <mergeCell ref="C2:H2"/>
     <mergeCell ref="A4:A15"/>
     <mergeCell ref="A16:A20"/>
-    <mergeCell ref="A21:A34"/>
+    <mergeCell ref="A21:A35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>